<commit_message>
started redoing ids #1
</commit_message>
<xml_diff>
--- a/database_schema.xlsx
+++ b/database_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherbaier/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherbaier/Documents/geo_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E519B19-85CE-344B-A47F-B706EAC10147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A36D0F-C851-7944-8AD5-F77FDC649D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16000" xr2:uid="{F2CB93DE-01A2-C84A-9FCD-7340BD7A8A45}"/>
+    <workbookView xWindow="220" yWindow="800" windowWidth="28040" windowHeight="16000" xr2:uid="{F2CB93DE-01A2-C84A-9FCD-7340BD7A8A45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,14 +90,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>186559</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>18641</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>402459</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>96603</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -112,8 +112,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7582441" y="3465784"/>
-          <a:ext cx="2681194" cy="1497374"/>
+          <a:off x="7616059" y="3219040"/>
+          <a:ext cx="2692400" cy="1835560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -175,6 +175,45 @@
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>school_name</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>address</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>adm0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>adm1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>adm2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>adm3</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -259,7 +298,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>adress</a:t>
+            <a:t>address</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -772,15 +811,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>702536</xdr:colOff>
+      <xdr:colOff>704404</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>96052</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>705391</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>18641</xdr:rowOff>
+      <xdr:colOff>707259</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171040</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -798,8 +837,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8920183" y="2529329"/>
-          <a:ext cx="2855" cy="936455"/>
+          <a:off x="8959404" y="2534452"/>
+          <a:ext cx="2855" cy="684588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -834,13 +873,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>402459</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>70131</xdr:rowOff>
+      <xdr:rowOff>70132</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>474843</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>159009</xdr:rowOff>
+      <xdr:rowOff>72820</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -858,8 +897,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10263635" y="2908955"/>
-          <a:ext cx="894149" cy="1305516"/>
+          <a:off x="10308459" y="2914932"/>
+          <a:ext cx="897884" cy="1221888"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -892,13 +931,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>705391</xdr:colOff>
+      <xdr:colOff>707259</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>96603</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>25487</xdr:colOff>
+      <xdr:colOff>23620</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>129589</xdr:rowOff>
     </xdr:to>
@@ -918,8 +957,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="8923038" y="4963158"/>
-          <a:ext cx="2607155" cy="438532"/>
+          <a:off x="8962259" y="5054600"/>
+          <a:ext cx="2618361" cy="358189"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -952,13 +991,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>71164</xdr:colOff>
+      <xdr:colOff>69297</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>96603</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>705391</xdr:colOff>
+      <xdr:colOff>707259</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>196610</xdr:rowOff>
     </xdr:to>
@@ -978,8 +1017,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6645282" y="4963158"/>
-          <a:ext cx="2277756" cy="505553"/>
+          <a:off x="6673297" y="5054600"/>
+          <a:ext cx="2288962" cy="425210"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1014,13 +1053,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>655510</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>200430</xdr:rowOff>
+      <xdr:rowOff>200644</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>186559</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>159009</xdr:rowOff>
+      <xdr:rowOff>72820</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1038,8 +1077,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6407863" y="3039254"/>
-          <a:ext cx="1174578" cy="1175217"/>
+          <a:off x="6434010" y="3045444"/>
+          <a:ext cx="1182049" cy="1091376"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1372,7 +1411,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>